<commit_message>
cái này để comment
</commit_message>
<xml_diff>
--- a/bangluudulieu_tamthoiapp.xlsx
+++ b/bangluudulieu_tamthoiapp.xlsx
@@ -490,17 +490,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>43C01338_C</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>43C01338_C</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>43C01338_C</t>
+          <t>43H03217</t>
         </is>
       </c>
     </row>
@@ -512,17 +502,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>12:05:58 27/06/2024</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>12:05:58 27/06/2024</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2024-06-27T12:05:58</t>
+          <t>13:52:50 02/07/2024</t>
         </is>
       </c>
     </row>
@@ -534,16 +514,8 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>34 Km/h</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>34 Km/h</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>34</v>
+          <t>49 Km/h</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -560,14 +532,6 @@
           <t>km trong ngày</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>26,36 km</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>26.36</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -575,11 +539,6 @@
           <t>Dừng đỗ</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>8 lần</t>
-        </is>
-      </c>
       <c r="D11" s="2" t="inlineStr"/>
     </row>
     <row r="12">
@@ -593,11 +552,6 @@
           <t>Bật</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Bật</t>
-        </is>
-      </c>
       <c r="D12" s="2" t="inlineStr"/>
     </row>
     <row r="13">
@@ -611,11 +565,6 @@
           <t>Tắt</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Tắt</t>
-        </is>
-      </c>
       <c r="D13" s="2" t="inlineStr"/>
     </row>
     <row r="14">
@@ -626,17 +575,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Cầu Trà Khúc 2, P. Lê Hồng Phong, TP. Quảng Ngãi, Quảng Ngãi</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Cầu Trà Khúc 2, P. Lê Hồng Phong, TP. Quảng Ngãi, Quảng Ngãi</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Cầu Trà Khúc 2, P. Lê Hồng Phong, TP. Quảng Ngãi, Quảng Ngãi</t>
+          <t>Quốc Lộ 1A, X. Tam Anh Nam, H. Núi Thành, Quảng Nam</t>
         </is>
       </c>
     </row>
@@ -654,11 +593,6 @@
           <t>nhiên liệu</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>146/400L</t>
-        </is>
-      </c>
       <c r="D16" s="2" t="inlineStr"/>
     </row>
     <row r="17">
@@ -667,11 +601,6 @@
           <t>nhiệt độ</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Mất kết nối cảm biến</t>
-        </is>
-      </c>
       <c r="D17" s="2" t="inlineStr"/>
     </row>
     <row r="18">
@@ -692,11 +621,6 @@
           <t>Số sim</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>0826585408</t>
-        </is>
-      </c>
       <c r="D19" s="2" t="inlineStr"/>
     </row>
     <row r="20">
@@ -705,11 +629,6 @@
           <t>Ngày đăng ký</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>09/05/2021</t>
-        </is>
-      </c>
       <c r="D20" s="2" t="inlineStr"/>
     </row>
     <row r="21">
@@ -718,11 +637,6 @@
           <t>Imei</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>868133049070873</t>
-        </is>
-      </c>
       <c r="D21" s="2" t="inlineStr"/>
     </row>
     <row r="22">
@@ -731,11 +645,6 @@
           <t>Km tích lũy</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>0 km</t>
-        </is>
-      </c>
       <c r="D22" s="2" t="inlineStr"/>
     </row>
     <row r="23">
@@ -744,11 +653,6 @@
           <t>Số lần mở cửa</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="D23" s="2" t="inlineStr"/>
     </row>
     <row r="24">
@@ -757,11 +661,6 @@
           <t>Thẻ nhớ</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Bình thường</t>
-        </is>
-      </c>
       <c r="D24" s="2" t="inlineStr"/>
     </row>
     <row r="25">
@@ -770,11 +669,6 @@
           <t>Nhóm đội</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>VICONSHIPCAM</t>
-        </is>
-      </c>
       <c r="D25" s="2" t="inlineStr"/>
     </row>
     <row r="26">
@@ -783,16 +677,6 @@
           <t>lái xe</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>PHAM THANH THUAN</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>PHAM THANH THUAN</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -800,16 +684,6 @@
           <t>bằng lái</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>48166002843</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>48166002843</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -825,14 +699,6 @@
           <t>thời gian lái xe liên tục</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>5 phút</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -840,14 +706,6 @@
           <t>thời gian lái xe trong ngày</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>31 phút</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>31</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -855,14 +713,6 @@
           <t>số lần quá tốc độ</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>0 lần</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -900,11 +750,6 @@
           <t>Vin</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>58251325</t>
-        </is>
-      </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="inlineStr">
@@ -912,11 +757,6 @@
           <t>tên gói cước</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>SCVINAQCB010</t>
-        </is>
-      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
@@ -924,11 +764,6 @@
           <t>nhà mạng</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Vina</t>
-        </is>
-      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
@@ -936,11 +771,6 @@
           <t>dung lượng gói cước</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>10240 MB</t>
-        </is>
-      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -948,11 +778,6 @@
           <t>Số ngày lưu trữ</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>0 ngày</t>
-        </is>
-      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
@@ -960,11 +785,6 @@
           <t>Số kênh lưu trữ</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -974,12 +794,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Danh sách phương tiện</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Có</t>
+          <t>Tổng số xe</t>
         </is>
       </c>
     </row>
@@ -991,12 +806,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Chuyển tới trang "Phương tiện"</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Có</t>
+          <t>Tổng các trạng thái</t>
         </is>
       </c>
     </row>
@@ -1006,11 +816,6 @@
           <t>tính năng video</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Có</t>
-        </is>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1018,21 +823,11 @@
           <t>Kênh lắp camera</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>1,2</t>
-        </is>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
           <t>Kênh hoạt động</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>1,2</t>
         </is>
       </c>
     </row>

</xml_diff>